<commit_message>
Add scale variables correlation table, additional variables cleanning
</commit_message>
<xml_diff>
--- a/var_description.xlsx
+++ b/var_description.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17766"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -14,12 +14,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">var_status!$A$1:$I$75</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="353">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="364">
   <si>
     <t>id</t>
   </si>
@@ -952,9 +952,6 @@
     <t>True = 문서길이, False = 0</t>
   </si>
   <si>
-    <t>15개 범주 = {1:15} (1부터 15까지)</t>
-  </si>
-  <si>
     <t>Number of derogatory public records</t>
   </si>
   <si>
@@ -1117,9 +1114,6 @@
     <t>지난 6 개월 간 신용관련 문의 건수 (자동차, 모기지 제외)</t>
   </si>
   <si>
-    <t>차용인의 여신 한도</t>
-  </si>
-  <si>
     <t>리볼빙 이용률, 차용자가 사용하는 리볼빙 크레딧 금액</t>
   </si>
   <si>
@@ -1183,10 +1177,62 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
+    <t>14개 범주 = {1:14} (1부터 14까지)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>차용인의 개설된 신용계좌 수</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>x</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>total_acc에 종속</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>loan_amnt에 종속</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>V1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>V2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>V3</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>V4</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>V5</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>V6</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>V18</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>V19</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
+    <t>V20</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>V21</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -1195,14 +1241,14 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>V24</t>
+    <t>V23</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1383,6 +1429,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -1430,7 +1479,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1463,9 +1512,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1498,6 +1564,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1677,7 +1760,7 @@
   <dimension ref="A1:I75"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1725,7 +1808,7 @@
     </row>
     <row r="2" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="15" t="s">
-        <v>290</v>
+        <v>352</v>
       </c>
       <c r="B2" s="15" t="s">
         <v>16</v>
@@ -1737,7 +1820,7 @@
         <v>260</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="F2" s="16">
         <v>1</v>
@@ -1752,7 +1835,7 @@
     </row>
     <row r="3" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">
-        <v>291</v>
+        <v>353</v>
       </c>
       <c r="B3" s="15" t="s">
         <v>5</v>
@@ -1772,12 +1855,12 @@
         <v>145</v>
       </c>
       <c r="I3" s="17" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="15" t="s">
-        <v>292</v>
+        <v>354</v>
       </c>
       <c r="B4" s="15" t="s">
         <v>6</v>
@@ -1802,24 +1885,26 @@
     </row>
     <row r="5" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="15" t="s">
-        <v>293</v>
+        <v>355</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C5" s="15" t="s">
         <v>273</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="E5" s="15"/>
+        <v>260</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>276</v>
+      </c>
       <c r="F5" s="16">
         <v>1</v>
       </c>
       <c r="G5" s="15"/>
       <c r="H5" s="17" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="I5" s="17" t="s">
         <v>318</v>
@@ -1827,10 +1912,10 @@
     </row>
     <row r="6" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="15" t="s">
-        <v>294</v>
+        <v>356</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C6" s="15" t="s">
         <v>273</v>
@@ -1839,25 +1924,25 @@
         <v>260</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="F6" s="16">
         <v>1</v>
       </c>
       <c r="G6" s="15"/>
       <c r="H6" s="17" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="I6" s="17" t="s">
-        <v>319</v>
+        <v>278</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="15" t="s">
-        <v>295</v>
+        <v>357</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C7" s="15" t="s">
         <v>273</v>
@@ -1866,17 +1951,17 @@
         <v>260</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="F7" s="16">
-        <v>1</v>
+        <v>0.94201237577179542</v>
       </c>
       <c r="G7" s="15"/>
       <c r="H7" s="17" t="s">
-        <v>150</v>
+        <v>116</v>
       </c>
       <c r="I7" s="17" t="s">
-        <v>278</v>
+        <v>319</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -1884,7 +1969,7 @@
         <v>296</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C8" s="15" t="s">
         <v>273</v>
@@ -1893,14 +1978,14 @@
         <v>260</v>
       </c>
       <c r="E8" s="15" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="F8" s="16">
-        <v>0.94201237577179542</v>
+        <v>1</v>
       </c>
       <c r="G8" s="15"/>
       <c r="H8" s="17" t="s">
-        <v>116</v>
+        <v>151</v>
       </c>
       <c r="I8" s="17" t="s">
         <v>320</v>
@@ -1911,7 +1996,7 @@
         <v>297</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C9" s="15" t="s">
         <v>273</v>
@@ -1920,14 +2005,14 @@
         <v>260</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>280</v>
+        <v>339</v>
       </c>
       <c r="F9" s="16">
         <v>1</v>
       </c>
       <c r="G9" s="15"/>
       <c r="H9" s="17" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="I9" s="17" t="s">
         <v>321</v>
@@ -1938,23 +2023,21 @@
         <v>298</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C10" s="15" t="s">
         <v>273</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>260</v>
-      </c>
-      <c r="E10" s="15" t="s">
-        <v>341</v>
-      </c>
+        <v>261</v>
+      </c>
+      <c r="E10" s="15"/>
       <c r="F10" s="16">
-        <v>1</v>
+        <v>0.99999549234318141</v>
       </c>
       <c r="G10" s="15"/>
       <c r="H10" s="17" t="s">
-        <v>152</v>
+        <v>132</v>
       </c>
       <c r="I10" s="17" t="s">
         <v>322</v>
@@ -1965,21 +2048,23 @@
         <v>299</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C11" s="15" t="s">
         <v>273</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="E11" s="15"/>
+        <v>260</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>281</v>
+      </c>
       <c r="F11" s="16">
-        <v>0.99999549234318141</v>
+        <v>1</v>
       </c>
       <c r="G11" s="15"/>
       <c r="H11" s="17" t="s">
-        <v>132</v>
+        <v>153</v>
       </c>
       <c r="I11" s="17" t="s">
         <v>323</v>
@@ -1990,7 +2075,7 @@
         <v>300</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C12" s="15" t="s">
         <v>273</v>
@@ -1999,17 +2084,17 @@
         <v>260</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="F12" s="16">
         <v>1</v>
       </c>
       <c r="G12" s="15"/>
       <c r="H12" s="17" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="I12" s="17" t="s">
-        <v>324</v>
+        <v>155</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -2017,34 +2102,31 @@
         <v>301</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="C13" s="15" t="s">
         <v>273</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>260</v>
-      </c>
-      <c r="E13" s="15" t="s">
-        <v>282</v>
-      </c>
+        <v>261</v>
+      </c>
+      <c r="E13" s="15"/>
       <c r="F13" s="16">
         <v>1</v>
       </c>
-      <c r="G13" s="15"/>
       <c r="H13" s="17" t="s">
-        <v>154</v>
+        <v>274</v>
       </c>
       <c r="I13" s="17" t="s">
-        <v>155</v>
+        <v>275</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="15" t="s">
-        <v>302</v>
+        <v>343</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="C14" s="15" t="s">
         <v>273</v>
@@ -2052,39 +2134,42 @@
       <c r="D14" s="15" t="s">
         <v>261</v>
       </c>
-      <c r="E14" s="15"/>
+      <c r="E14" s="15" t="s">
+        <v>284</v>
+      </c>
       <c r="F14" s="16">
-        <v>1</v>
-      </c>
+        <v>0.14202499721088735</v>
+      </c>
+      <c r="G14" s="15"/>
       <c r="H14" s="17" t="s">
-        <v>274</v>
+        <v>103</v>
       </c>
       <c r="I14" s="17" t="s">
-        <v>275</v>
+        <v>325</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="15" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C15" s="15" t="s">
         <v>273</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E15" s="15" t="s">
-        <v>284</v>
+        <v>347</v>
       </c>
       <c r="F15" s="16">
-        <v>0.14202499721088735</v>
+        <v>1</v>
       </c>
       <c r="G15" s="15"/>
       <c r="H15" s="17" t="s">
-        <v>103</v>
+        <v>159</v>
       </c>
       <c r="I15" s="17" t="s">
         <v>326</v>
@@ -2092,26 +2177,24 @@
     </row>
     <row r="16" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="15" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C16" s="15" t="s">
         <v>273</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>260</v>
-      </c>
-      <c r="E16" s="15" t="s">
-        <v>285</v>
-      </c>
+        <v>261</v>
+      </c>
+      <c r="E16" s="15"/>
       <c r="F16" s="16">
         <v>1</v>
       </c>
       <c r="G16" s="15"/>
       <c r="H16" s="17" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="I16" s="17" t="s">
         <v>327</v>
@@ -2119,10 +2202,10 @@
     </row>
     <row r="17" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="15" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C17" s="15" t="s">
         <v>273</v>
@@ -2132,11 +2215,11 @@
       </c>
       <c r="E17" s="15"/>
       <c r="F17" s="16">
-        <v>1</v>
+        <v>0.99996731948806539</v>
       </c>
       <c r="G17" s="15"/>
       <c r="H17" s="17" t="s">
-        <v>164</v>
+        <v>127</v>
       </c>
       <c r="I17" s="17" t="s">
         <v>328</v>
@@ -2144,10 +2227,10 @@
     </row>
     <row r="18" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="15" t="s">
-        <v>348</v>
+        <v>306</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C18" s="15" t="s">
         <v>273</v>
@@ -2157,11 +2240,11 @@
       </c>
       <c r="E18" s="15"/>
       <c r="F18" s="16">
-        <v>0.99996731948806539</v>
+        <v>1</v>
       </c>
       <c r="G18" s="15"/>
       <c r="H18" s="17" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="I18" s="17" t="s">
         <v>329</v>
@@ -2169,10 +2252,10 @@
     </row>
     <row r="19" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="15" t="s">
-        <v>307</v>
+        <v>358</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C19" s="15" t="s">
         <v>273</v>
@@ -2182,22 +2265,22 @@
       </c>
       <c r="E19" s="15"/>
       <c r="F19" s="16">
-        <v>1</v>
+        <v>0.99996731948806539</v>
       </c>
       <c r="G19" s="15"/>
       <c r="H19" s="17" t="s">
-        <v>125</v>
+        <v>285</v>
       </c>
       <c r="I19" s="17" t="s">
-        <v>330</v>
+        <v>286</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="15" t="s">
-        <v>308</v>
+        <v>359</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C20" s="15" t="s">
         <v>273</v>
@@ -2207,22 +2290,22 @@
       </c>
       <c r="E20" s="15"/>
       <c r="F20" s="16">
-        <v>0.99996731948806539</v>
+        <v>1</v>
       </c>
       <c r="G20" s="15"/>
       <c r="H20" s="17" t="s">
-        <v>130</v>
+        <v>165</v>
       </c>
       <c r="I20" s="17" t="s">
-        <v>331</v>
+        <v>166</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="15" t="s">
-        <v>349</v>
+        <v>360</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C21" s="15" t="s">
         <v>273</v>
@@ -2232,22 +2315,22 @@
       </c>
       <c r="E21" s="15"/>
       <c r="F21" s="16">
-        <v>0.99996731948806539</v>
+        <v>0.99943428906927034</v>
       </c>
       <c r="G21" s="15"/>
       <c r="H21" s="17" t="s">
-        <v>286</v>
+        <v>119</v>
       </c>
       <c r="I21" s="17" t="s">
-        <v>287</v>
+        <v>330</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="15" t="s">
-        <v>310</v>
+        <v>361</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C22" s="15" t="s">
         <v>273</v>
@@ -2257,36 +2340,38 @@
       </c>
       <c r="E22" s="15"/>
       <c r="F22" s="16">
-        <v>1</v>
+        <v>0.99996731948806539</v>
       </c>
       <c r="G22" s="15"/>
       <c r="H22" s="17" t="s">
-        <v>165</v>
+        <v>131</v>
       </c>
       <c r="I22" s="17" t="s">
-        <v>166</v>
+        <v>331</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="15" t="s">
-        <v>350</v>
+        <v>362</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C23" s="15" t="s">
         <v>273</v>
       </c>
       <c r="D23" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="E23" s="15"/>
+        <v>260</v>
+      </c>
+      <c r="E23" s="15" t="s">
+        <v>287</v>
+      </c>
       <c r="F23" s="16">
-        <v>0.99943428906927034</v>
+        <v>1</v>
       </c>
       <c r="G23" s="15"/>
       <c r="H23" s="17" t="s">
-        <v>119</v>
+        <v>167</v>
       </c>
       <c r="I23" s="17" t="s">
         <v>332</v>
@@ -2294,10 +2379,10 @@
     </row>
     <row r="24" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="15" t="s">
-        <v>351</v>
+        <v>363</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
       <c r="C24" s="15" t="s">
         <v>273</v>
@@ -2307,72 +2392,70 @@
       </c>
       <c r="E24" s="15"/>
       <c r="F24" s="16">
-        <v>0.99996731948806539</v>
+        <v>0.99996619257386077</v>
       </c>
       <c r="G24" s="15"/>
       <c r="H24" s="17" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="I24" s="17" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="15" t="s">
-        <v>313</v>
-      </c>
+      <c r="A25" s="15"/>
       <c r="B25" s="15" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>273</v>
+        <v>192</v>
       </c>
       <c r="D25" s="15" t="s">
-        <v>260</v>
-      </c>
-      <c r="E25" s="15" t="s">
-        <v>288</v>
-      </c>
-      <c r="F25" s="16">
-        <v>1</v>
-      </c>
-      <c r="G25" s="15"/>
+        <v>208</v>
+      </c>
+      <c r="E25" s="15"/>
+      <c r="F25" s="20">
+        <v>1</v>
+      </c>
+      <c r="G25" s="19" t="s">
+        <v>202</v>
+      </c>
       <c r="H25" s="17" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="I25" s="17" t="s">
-        <v>334</v>
+        <v>163</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="15" t="s">
-        <v>352</v>
-      </c>
+      <c r="A26" s="15"/>
       <c r="B26" s="15" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>273</v>
+        <v>192</v>
       </c>
       <c r="D26" s="15" t="s">
-        <v>261</v>
+        <v>208</v>
       </c>
       <c r="E26" s="15"/>
-      <c r="F26" s="16">
-        <v>0.99996619257386077</v>
-      </c>
-      <c r="G26" s="15"/>
+      <c r="F26" s="20">
+        <v>2.4085537295789061E-2</v>
+      </c>
+      <c r="G26" s="15" t="s">
+        <v>206</v>
+      </c>
       <c r="H26" s="17" t="s">
-        <v>126</v>
+        <v>101</v>
       </c>
       <c r="I26" s="17" t="s">
-        <v>336</v>
+        <v>102</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="15"/>
       <c r="B27" s="15" t="s">
-        <v>23</v>
+        <v>52</v>
       </c>
       <c r="C27" s="15" t="s">
         <v>192</v>
@@ -2382,247 +2465,247 @@
       </c>
       <c r="E27" s="15"/>
       <c r="F27" s="20">
-        <v>1</v>
-      </c>
-      <c r="G27" s="19" t="s">
-        <v>202</v>
+        <v>5.7585315857147852E-4</v>
+      </c>
+      <c r="G27" s="15" t="s">
+        <v>205</v>
       </c>
       <c r="H27" s="17" t="s">
-        <v>162</v>
+        <v>79</v>
       </c>
       <c r="I27" s="17" t="s">
-        <v>163</v>
+        <v>80</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="15"/>
       <c r="B28" s="15" t="s">
-        <v>68</v>
+        <v>51</v>
       </c>
       <c r="C28" s="15" t="s">
-        <v>192</v>
+        <v>340</v>
       </c>
       <c r="D28" s="15" t="s">
-        <v>208</v>
-      </c>
-      <c r="E28" s="15"/>
-      <c r="F28" s="20">
-        <v>2.4085537295789061E-2</v>
+        <v>260</v>
+      </c>
+      <c r="E28" s="15" t="s">
+        <v>288</v>
+      </c>
+      <c r="F28" s="16">
+        <v>0.99999774617159076</v>
       </c>
       <c r="G28" s="15" t="s">
-        <v>206</v>
+        <v>341</v>
       </c>
       <c r="H28" s="17" t="s">
-        <v>101</v>
+        <v>133</v>
       </c>
       <c r="I28" s="17" t="s">
-        <v>102</v>
+        <v>333</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="15"/>
       <c r="B29" s="15" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="C29" s="15" t="s">
         <v>192</v>
       </c>
       <c r="D29" s="15" t="s">
-        <v>208</v>
+        <v>261</v>
       </c>
       <c r="E29" s="15"/>
       <c r="F29" s="20">
-        <v>5.7585315857147852E-4</v>
+        <v>1</v>
       </c>
       <c r="G29" s="15" t="s">
-        <v>205</v>
+        <v>267</v>
       </c>
       <c r="H29" s="17" t="s">
-        <v>79</v>
+        <v>182</v>
       </c>
       <c r="I29" s="17" t="s">
-        <v>80</v>
+        <v>183</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="15"/>
       <c r="B30" s="15" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>342</v>
+        <v>266</v>
       </c>
       <c r="D30" s="15" t="s">
-        <v>260</v>
-      </c>
-      <c r="E30" s="15" t="s">
-        <v>289</v>
-      </c>
-      <c r="F30" s="16">
-        <v>0.99999774617159076</v>
+        <v>261</v>
+      </c>
+      <c r="E30" s="15"/>
+      <c r="F30" s="20">
+        <v>0.99983434361191781</v>
       </c>
       <c r="G30" s="15" t="s">
-        <v>343</v>
+        <v>268</v>
       </c>
       <c r="H30" s="17" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="I30" s="17" t="s">
-        <v>335</v>
+        <v>123</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="15"/>
       <c r="B31" s="15" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="C31" s="15" t="s">
         <v>192</v>
       </c>
       <c r="D31" s="15" t="s">
-        <v>261</v>
+        <v>208</v>
       </c>
       <c r="E31" s="15"/>
       <c r="F31" s="20">
-        <v>1</v>
-      </c>
-      <c r="G31" s="15" t="s">
-        <v>267</v>
-      </c>
+        <v>5.7359933016219678E-4</v>
+      </c>
+      <c r="G31" s="15"/>
       <c r="H31" s="17" t="s">
-        <v>182</v>
+        <v>77</v>
       </c>
       <c r="I31" s="17" t="s">
-        <v>183</v>
+        <v>78</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="15"/>
       <c r="B32" s="15" t="s">
-        <v>48</v>
+        <v>26</v>
       </c>
       <c r="C32" s="15" t="s">
-        <v>266</v>
+        <v>192</v>
       </c>
       <c r="D32" s="15" t="s">
-        <v>261</v>
+        <v>243</v>
       </c>
       <c r="E32" s="15"/>
       <c r="F32" s="20">
-        <v>0.99983434361191781</v>
+        <v>0.99996731948806539</v>
       </c>
       <c r="G32" s="15" t="s">
-        <v>268</v>
+        <v>244</v>
       </c>
       <c r="H32" s="17" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="I32" s="17" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="15"/>
       <c r="B33" s="15" t="s">
-        <v>53</v>
+        <v>3</v>
       </c>
       <c r="C33" s="15" t="s">
         <v>192</v>
       </c>
       <c r="D33" s="15" t="s">
-        <v>208</v>
+        <v>261</v>
       </c>
       <c r="E33" s="15"/>
       <c r="F33" s="20">
-        <v>5.7359933016219678E-4</v>
-      </c>
-      <c r="G33" s="15"/>
+        <v>1</v>
+      </c>
+      <c r="G33" s="15" t="s">
+        <v>262</v>
+      </c>
       <c r="H33" s="17" t="s">
-        <v>77</v>
+        <v>142</v>
       </c>
       <c r="I33" s="17" t="s">
-        <v>78</v>
+        <v>143</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="15"/>
       <c r="B34" s="15" t="s">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="C34" s="15" t="s">
         <v>192</v>
       </c>
       <c r="D34" s="15" t="s">
-        <v>243</v>
+        <v>261</v>
       </c>
       <c r="E34" s="15"/>
       <c r="F34" s="20">
-        <v>0.99996731948806539</v>
+        <v>1</v>
       </c>
       <c r="G34" s="15" t="s">
-        <v>244</v>
+        <v>263</v>
       </c>
       <c r="H34" s="17" t="s">
-        <v>128</v>
+        <v>144</v>
       </c>
       <c r="I34" s="17" t="s">
-        <v>129</v>
+        <v>258</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="15"/>
       <c r="B35" s="15" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C35" s="15" t="s">
         <v>192</v>
       </c>
       <c r="D35" s="15" t="s">
-        <v>261</v>
+        <v>208</v>
       </c>
       <c r="E35" s="15"/>
       <c r="F35" s="20">
         <v>1</v>
       </c>
-      <c r="G35" s="15" t="s">
-        <v>262</v>
+      <c r="G35" s="19" t="s">
+        <v>204</v>
       </c>
       <c r="H35" s="17" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="I35" s="17" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="15"/>
       <c r="B36" s="15" t="s">
-        <v>4</v>
+        <v>64</v>
       </c>
       <c r="C36" s="15" t="s">
         <v>192</v>
       </c>
       <c r="D36" s="15" t="s">
-        <v>261</v>
+        <v>208</v>
       </c>
       <c r="E36" s="15"/>
       <c r="F36" s="20">
-        <v>1</v>
+        <v>2.0979761747798854E-2</v>
       </c>
       <c r="G36" s="15" t="s">
-        <v>263</v>
+        <v>206</v>
       </c>
       <c r="H36" s="17" t="s">
-        <v>144</v>
+        <v>81</v>
       </c>
       <c r="I36" s="17" t="s">
-        <v>258</v>
+        <v>82</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="15"/>
       <c r="B37" s="15" t="s">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="C37" s="15" t="s">
         <v>192</v>
@@ -2632,47 +2715,47 @@
       </c>
       <c r="E37" s="15"/>
       <c r="F37" s="20">
-        <v>1</v>
-      </c>
-      <c r="G37" s="19" t="s">
-        <v>204</v>
+        <v>0</v>
+      </c>
+      <c r="G37" s="15" t="s">
+        <v>206</v>
       </c>
       <c r="H37" s="17" t="s">
-        <v>138</v>
+        <v>186</v>
       </c>
       <c r="I37" s="17" t="s">
-        <v>139</v>
+        <v>187</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="15"/>
       <c r="B38" s="15" t="s">
-        <v>64</v>
+        <v>7</v>
       </c>
       <c r="C38" s="15" t="s">
-        <v>192</v>
+        <v>349</v>
       </c>
       <c r="D38" s="15" t="s">
-        <v>208</v>
+        <v>261</v>
       </c>
       <c r="E38" s="15"/>
-      <c r="F38" s="20">
-        <v>2.0979761747798854E-2</v>
+      <c r="F38" s="16">
+        <v>1</v>
       </c>
       <c r="G38" s="15" t="s">
-        <v>206</v>
+        <v>351</v>
       </c>
       <c r="H38" s="17" t="s">
-        <v>81</v>
+        <v>148</v>
       </c>
       <c r="I38" s="17" t="s">
-        <v>82</v>
+        <v>317</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="15"/>
       <c r="B39" s="15" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C39" s="15" t="s">
         <v>192</v>
@@ -2688,164 +2771,164 @@
         <v>206</v>
       </c>
       <c r="H39" s="17" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="I39" s="17" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="15"/>
       <c r="B40" s="15" t="s">
-        <v>72</v>
+        <v>47</v>
       </c>
       <c r="C40" s="15" t="s">
         <v>192</v>
       </c>
-      <c r="D40" s="15" t="s">
-        <v>208</v>
-      </c>
+      <c r="D40" s="15"/>
       <c r="E40" s="15"/>
       <c r="F40" s="20">
-        <v>0</v>
+        <v>0.99994027354715398</v>
       </c>
       <c r="G40" s="15" t="s">
-        <v>206</v>
+        <v>245</v>
       </c>
       <c r="H40" s="17" t="s">
-        <v>190</v>
+        <v>124</v>
       </c>
       <c r="I40" s="17" t="s">
-        <v>191</v>
+        <v>209</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="15"/>
       <c r="B41" s="15" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C41" s="15" t="s">
         <v>192</v>
       </c>
-      <c r="D41" s="15"/>
+      <c r="D41" s="15" t="s">
+        <v>261</v>
+      </c>
       <c r="E41" s="15"/>
       <c r="F41" s="20">
-        <v>0.99994027354715398</v>
+        <v>0.99999887308579538</v>
       </c>
       <c r="G41" s="15" t="s">
-        <v>245</v>
+        <v>270</v>
       </c>
       <c r="H41" s="17" t="s">
-        <v>124</v>
+        <v>136</v>
       </c>
       <c r="I41" s="17" t="s">
-        <v>209</v>
+        <v>137</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="15"/>
       <c r="B42" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C42" s="15" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="D42" s="15" t="s">
-        <v>261</v>
+        <v>210</v>
       </c>
       <c r="E42" s="15"/>
       <c r="F42" s="20">
-        <v>0.99999887308579538</v>
+        <v>0.98009982206024704</v>
       </c>
       <c r="G42" s="15" t="s">
-        <v>270</v>
+        <v>203</v>
       </c>
       <c r="H42" s="17" t="s">
-        <v>136</v>
+        <v>117</v>
       </c>
       <c r="I42" s="17" t="s">
-        <v>137</v>
+        <v>118</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="15"/>
       <c r="B43" s="15" t="s">
-        <v>44</v>
+        <v>67</v>
       </c>
       <c r="C43" s="15" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D43" s="15" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="E43" s="15"/>
       <c r="F43" s="20">
-        <v>0.98009982206024704</v>
+        <v>2.4084410381584417E-2</v>
       </c>
       <c r="G43" s="15" t="s">
-        <v>203</v>
+        <v>212</v>
       </c>
       <c r="H43" s="17" t="s">
-        <v>117</v>
+        <v>99</v>
       </c>
       <c r="I43" s="17" t="s">
-        <v>118</v>
+        <v>100</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="15"/>
       <c r="B44" s="15" t="s">
-        <v>67</v>
+        <v>1</v>
       </c>
       <c r="C44" s="15" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D44" s="15" t="s">
         <v>211</v>
       </c>
       <c r="E44" s="15"/>
       <c r="F44" s="20">
-        <v>2.4084410381584417E-2</v>
-      </c>
-      <c r="G44" s="15" t="s">
-        <v>212</v>
+        <v>1</v>
+      </c>
+      <c r="G44" s="19" t="s">
+        <v>213</v>
       </c>
       <c r="H44" s="17" t="s">
-        <v>99</v>
+        <v>140</v>
       </c>
       <c r="I44" s="17" t="s">
-        <v>100</v>
+        <v>141</v>
       </c>
     </row>
     <row r="45" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="15"/>
       <c r="B45" s="15" t="s">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="C45" s="15" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D45" s="15" t="s">
         <v>211</v>
       </c>
       <c r="E45" s="15"/>
       <c r="F45" s="20">
-        <v>1</v>
-      </c>
-      <c r="G45" s="19" t="s">
-        <v>213</v>
+        <v>0.48802822694699782</v>
+      </c>
+      <c r="G45" s="15" t="s">
+        <v>214</v>
       </c>
       <c r="H45" s="17" t="s">
-        <v>140</v>
+        <v>108</v>
       </c>
       <c r="I45" s="17" t="s">
-        <v>141</v>
+        <v>109</v>
       </c>
     </row>
     <row r="46" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="15"/>
       <c r="B46" s="15" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="C46" s="15" t="s">
         <v>192</v>
@@ -2855,22 +2938,22 @@
       </c>
       <c r="E46" s="15"/>
       <c r="F46" s="20">
-        <v>0.48802822694699782</v>
+        <v>0.24984251373990143</v>
       </c>
       <c r="G46" s="15" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="H46" s="17" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="I46" s="17" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="47" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="15"/>
       <c r="B47" s="15" t="s">
-        <v>49</v>
+        <v>29</v>
       </c>
       <c r="C47" s="15" t="s">
         <v>192</v>
@@ -2880,22 +2963,22 @@
       </c>
       <c r="E47" s="15"/>
       <c r="F47" s="20">
-        <v>0.24984251373990143</v>
+        <v>0.1544492263170528</v>
       </c>
       <c r="G47" s="15" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="H47" s="17" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="I47" s="17" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="48" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="15"/>
       <c r="B48" s="15" t="s">
-        <v>29</v>
+        <v>62</v>
       </c>
       <c r="C48" s="15" t="s">
         <v>192</v>
@@ -2905,22 +2988,22 @@
       </c>
       <c r="E48" s="15"/>
       <c r="F48" s="20">
-        <v>0.1544492263170528</v>
+        <v>2.3451084598576255E-2</v>
       </c>
       <c r="G48" s="15" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H48" s="17" t="s">
-        <v>104</v>
+        <v>83</v>
       </c>
       <c r="I48" s="17" t="s">
-        <v>105</v>
+        <v>84</v>
       </c>
     </row>
     <row r="49" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="15"/>
       <c r="B49" s="15" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="C49" s="15" t="s">
         <v>192</v>
@@ -2930,41 +3013,41 @@
       </c>
       <c r="E49" s="15"/>
       <c r="F49" s="20">
-        <v>2.3451084598576255E-2</v>
-      </c>
-      <c r="G49" s="15" t="s">
-        <v>215</v>
+        <v>0.71492451365200216</v>
+      </c>
+      <c r="G49" s="19" t="s">
+        <v>214</v>
       </c>
       <c r="H49" s="17" t="s">
-        <v>83</v>
+        <v>110</v>
       </c>
       <c r="I49" s="17" t="s">
-        <v>84</v>
+        <v>111</v>
       </c>
     </row>
     <row r="50" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="15"/>
       <c r="B50" s="15" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="C50" s="15" t="s">
         <v>192</v>
       </c>
       <c r="D50" s="15" t="s">
-        <v>211</v>
+        <v>261</v>
       </c>
       <c r="E50" s="15"/>
-      <c r="F50" s="20">
-        <v>0.71492451365200216</v>
-      </c>
-      <c r="G50" s="19" t="s">
-        <v>214</v>
+      <c r="F50" s="16">
+        <v>0.99996731948806539</v>
+      </c>
+      <c r="G50" s="15" t="s">
+        <v>350</v>
       </c>
       <c r="H50" s="17" t="s">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="I50" s="17" t="s">
-        <v>111</v>
+        <v>348</v>
       </c>
     </row>
     <row r="51" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -3198,7 +3281,7 @@
         <v>17</v>
       </c>
       <c r="C60" s="15" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="D60" s="15" t="s">
         <v>260</v>
@@ -3210,13 +3293,13 @@
         <v>1</v>
       </c>
       <c r="G60" s="15" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="H60" s="17" t="s">
         <v>158</v>
       </c>
       <c r="I60" s="17" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="61" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -3553,7 +3636,7 @@
         <v>192</v>
       </c>
       <c r="D74" s="15" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="E74" s="15"/>
       <c r="F74" s="20">
@@ -3606,7 +3689,7 @@
   <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3618,7 +3701,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>256</v>
@@ -3724,7 +3807,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>257</v>
@@ -3969,85 +4052,85 @@
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
+        <v>289</v>
+      </c>
+      <c r="B2" s="11" t="s">
         <v>290</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="C2" s="11" t="s">
         <v>291</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="D2" s="11" t="s">
         <v>292</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="E2" s="11" t="s">
         <v>293</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="F2" s="11" t="s">
         <v>294</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="G2" s="11" t="s">
         <v>295</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="H2" s="11" t="s">
         <v>296</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="I2" s="11" t="s">
         <v>297</v>
       </c>
-      <c r="I2" s="11" t="s">
+      <c r="J2" s="11" t="s">
         <v>298</v>
       </c>
-      <c r="J2" s="11" t="s">
+      <c r="K2" s="11" t="s">
         <v>299</v>
       </c>
-      <c r="K2" s="11" t="s">
+      <c r="L2" s="11" t="s">
         <v>300</v>
       </c>
-      <c r="L2" s="11" t="s">
+      <c r="M2" s="11" t="s">
         <v>301</v>
       </c>
-      <c r="M2" s="11" t="s">
+      <c r="N2" s="11" t="s">
         <v>302</v>
       </c>
-      <c r="N2" s="11" t="s">
+      <c r="O2" s="11" t="s">
         <v>303</v>
       </c>
-      <c r="O2" s="11" t="s">
+      <c r="P2" s="11" t="s">
         <v>304</v>
       </c>
-      <c r="P2" s="11" t="s">
+      <c r="Q2" s="11" t="s">
         <v>305</v>
       </c>
-      <c r="Q2" s="11" t="s">
+      <c r="R2" s="11" t="s">
         <v>306</v>
       </c>
-      <c r="R2" s="11" t="s">
+      <c r="S2" s="11" t="s">
         <v>307</v>
       </c>
-      <c r="S2" s="11" t="s">
+      <c r="T2" s="11" t="s">
         <v>308</v>
       </c>
-      <c r="T2" s="11" t="s">
+      <c r="U2" s="11" t="s">
         <v>309</v>
       </c>
-      <c r="U2" s="11" t="s">
+      <c r="V2" s="11" t="s">
         <v>310</v>
       </c>
-      <c r="V2" s="11" t="s">
+      <c r="W2" s="11" t="s">
         <v>311</v>
       </c>
-      <c r="W2" s="11" t="s">
+      <c r="X2" s="11" t="s">
         <v>312</v>
       </c>
-      <c r="X2" s="11" t="s">
+      <c r="Y2" s="11" t="s">
         <v>313</v>
       </c>
-      <c r="Y2" s="11" t="s">
+      <c r="Z2" s="11" t="s">
         <v>314</v>
       </c>
-      <c r="Z2" s="11" t="s">
+      <c r="AA2" s="11" t="s">
         <v>315</v>
-      </c>
-      <c r="AA2" s="11" t="s">
-        <v>316</v>
       </c>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
add plots, frames, and data cleaning
</commit_message>
<xml_diff>
--- a/var_description.xlsx
+++ b/var_description.xlsx
@@ -1145,10 +1145,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Mortgage, None, Other, Own, Rent = {1, 2, 3, 4, 5}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>x</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -1242,6 +1238,10 @@
   </si>
   <si>
     <t>V23</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mortgage, Other, Own, Rent = {1, 2, 3, 4}</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1760,7 +1760,7 @@
   <dimension ref="A1:I75"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1808,7 +1808,7 @@
     </row>
     <row r="2" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="15" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B2" s="15" t="s">
         <v>16</v>
@@ -1835,7 +1835,7 @@
     </row>
     <row r="3" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B3" s="15" t="s">
         <v>5</v>
@@ -1860,7 +1860,7 @@
     </row>
     <row r="4" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="15" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B4" s="15" t="s">
         <v>6</v>
@@ -1885,7 +1885,7 @@
     </row>
     <row r="5" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="15" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B5" s="15" t="s">
         <v>8</v>
@@ -1912,7 +1912,7 @@
     </row>
     <row r="6" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="15" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B6" s="15" t="s">
         <v>9</v>
@@ -1939,7 +1939,7 @@
     </row>
     <row r="7" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="15" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B7" s="15" t="s">
         <v>10</v>
@@ -2005,7 +2005,7 @@
         <v>260</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>339</v>
+        <v>363</v>
       </c>
       <c r="F9" s="16">
         <v>1</v>
@@ -2123,7 +2123,7 @@
     </row>
     <row r="14" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="15" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B14" s="15" t="s">
         <v>19</v>
@@ -2150,7 +2150,7 @@
     </row>
     <row r="15" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="15" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B15" s="15" t="s">
         <v>20</v>
@@ -2162,7 +2162,7 @@
         <v>260</v>
       </c>
       <c r="E15" s="15" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="F15" s="16">
         <v>1</v>
@@ -2177,7 +2177,7 @@
     </row>
     <row r="16" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="15" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B16" s="15" t="s">
         <v>24</v>
@@ -2202,7 +2202,7 @@
     </row>
     <row r="17" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="15" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B17" s="15" t="s">
         <v>25</v>
@@ -2252,7 +2252,7 @@
     </row>
     <row r="19" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="15" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B19" s="15" t="s">
         <v>31</v>
@@ -2277,7 +2277,7 @@
     </row>
     <row r="20" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="15" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B20" s="15" t="s">
         <v>32</v>
@@ -2302,7 +2302,7 @@
     </row>
     <row r="21" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="15" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B21" s="15" t="s">
         <v>33</v>
@@ -2327,7 +2327,7 @@
     </row>
     <row r="22" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="15" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B22" s="15" t="s">
         <v>34</v>
@@ -2352,7 +2352,7 @@
     </row>
     <row r="23" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="15" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B23" s="15" t="s">
         <v>35</v>
@@ -2379,7 +2379,7 @@
     </row>
     <row r="24" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="15" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B24" s="15" t="s">
         <v>55</v>
@@ -2483,7 +2483,7 @@
         <v>51</v>
       </c>
       <c r="C28" s="15" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D28" s="15" t="s">
         <v>260</v>
@@ -2495,7 +2495,7 @@
         <v>0.99999774617159076</v>
       </c>
       <c r="G28" s="15" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="H28" s="17" t="s">
         <v>133</v>
@@ -2733,7 +2733,7 @@
         <v>7</v>
       </c>
       <c r="C38" s="15" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D38" s="15" t="s">
         <v>261</v>
@@ -2743,7 +2743,7 @@
         <v>1</v>
       </c>
       <c r="G38" s="15" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="H38" s="17" t="s">
         <v>148</v>
@@ -3041,13 +3041,13 @@
         <v>0.99996731948806539</v>
       </c>
       <c r="G50" s="15" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H50" s="17" t="s">
         <v>130</v>
       </c>
       <c r="I50" s="17" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="51" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -3281,7 +3281,7 @@
         <v>17</v>
       </c>
       <c r="C60" s="15" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D60" s="15" t="s">
         <v>260</v>
@@ -3293,7 +3293,7 @@
         <v>1</v>
       </c>
       <c r="G60" s="15" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="H60" s="17" t="s">
         <v>158</v>

</xml_diff>